<commit_message>
perf(alu_64_bit_slim_withbr.v,-alu_64_bit_slim.v-and-tests-folder-that-holds-the-test-benches-for-these-modules): these modules have been tested oon modelsim. Analysis file has the details of the source utilization
</commit_message>
<xml_diff>
--- a/logs/analysis.xlsx
+++ b/logs/analysis.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Not Sycned\tools_notsynced\shared-ubuntu64_22-04\aurora\aurora\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04138251-22EB-46C3-9595-EA28E42E1553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D19534A-C504-426A-BBAD-131F89092606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF379C5B-85D5-4F73-801D-DB5F675D5241}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{DF379C5B-85D5-4F73-801D-DB5F675D5241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Resourceutilization" sheetId="2" r:id="rId2"/>
+    <sheet name="fedorsa_results" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$4:$E$165</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="301">
   <si>
     <t>Location             Delay type         Delay(ns)  Physical Resource</t>
   </si>
@@ -750,13 +752,205 @@
   </si>
   <si>
     <t>going to adder1, IDEX, bralu</t>
+  </si>
+  <si>
+    <t>Number of wires:                 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of wire bits:            796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of public wires:           7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of public wire bits:     270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of memories:               0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of memory bits:            0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of processes:              0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of cells:                 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $add                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $and                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $eq                             9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $logic_not                      1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $lt                             2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $mux                            2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $or                             1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $pmux                           1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $shl                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $shr                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $sshr                           1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $sub                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $xor                            1</t>
+  </si>
+  <si>
+    <t>alu_64_bit.v</t>
+  </si>
+  <si>
+    <t>=== alu_64_bit_slim ===</t>
+  </si>
+  <si>
+    <t>   Number of wires:                 33</t>
+  </si>
+  <si>
+    <t>   Number of wire bits:            794</t>
+  </si>
+  <si>
+    <t>   Number of public wires:          15</t>
+  </si>
+  <si>
+    <t>   Number of public wire bits:     398</t>
+  </si>
+  <si>
+    <t>   Number of memories:               0</t>
+  </si>
+  <si>
+    <t>   Number of memory bits:            0</t>
+  </si>
+  <si>
+    <t>   Number of processes:              0</t>
+  </si>
+  <si>
+    <t>   Number of cells:                 87</t>
+  </si>
+  <si>
+    <t>     $and                            1</t>
+  </si>
+  <si>
+    <t>     $eq                             9</t>
+  </si>
+  <si>
+    <t>     $logic_not                      1</t>
+  </si>
+  <si>
+    <t>     $mux                            1</t>
+  </si>
+  <si>
+    <t>     $not                            1</t>
+  </si>
+  <si>
+    <t>     $or                             1</t>
+  </si>
+  <si>
+    <t>     $pmux                           1</t>
+  </si>
+  <si>
+    <t>     $reduce_or                      2</t>
+  </si>
+  <si>
+    <t>     $shl                            1</t>
+  </si>
+  <si>
+    <t>     $shr                            1</t>
+  </si>
+  <si>
+    <t>     $sshr                           1</t>
+  </si>
+  <si>
+    <t>     $xor                            3</t>
+  </si>
+  <si>
+    <t>     structuraladd_sub              64</t>
+  </si>
+  <si>
+    <t>== structuraladd_sub ===</t>
+  </si>
+  <si>
+    <t>   Number of wires:                  9</t>
+  </si>
+  <si>
+    <t>   Number of wire bits:             10</t>
+  </si>
+  <si>
+    <t>   Number of public wires:           7</t>
+  </si>
+  <si>
+    <t>   Number of public wire bits:       7</t>
+  </si>
+  <si>
+    <t>   Number of cells:                  4</t>
+  </si>
+  <si>
+    <t>     $add                            2</t>
+  </si>
+  <si>
+    <t>Original ALU</t>
+  </si>
+  <si>
+    <t>Number of Slice Flip Flops:        14,097 out of  47,232   29%</t>
+  </si>
+  <si>
+    <t>Number of 4 input LUTs:            20,546 out of  47,232   43%</t>
+  </si>
+  <si>
+    <t>Number of occupied Slices:         14,986 out of  23,616   63%</t>
+  </si>
+  <si>
+    <t>Reference Router</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Number of Slice Flip Flops:        14,051 out of  47,232   29%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Number of 4 input LUTs:            21,114 out of  47,232   44%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Number of occupied Slices:         14,263 out of  23,616   60%</t>
+  </si>
+  <si>
+    <t>Modified ALU</t>
+  </si>
+  <si>
+    <t>ALU_withbranch</t>
+  </si>
+  <si>
+    <t>Ref Router + UDP</t>
+  </si>
+  <si>
+    <t>Number of 4 input LUTs:            20,543 out of  47,232   43%</t>
+  </si>
+  <si>
+    <t>Number of occupied Slices:         14,542 out of  23,616   61%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,13 +958,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -785,8 +991,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1103,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58415AEC-B408-4D3D-935C-9A3C607B29F3}">
   <dimension ref="B2:Z165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -2813,7 +3021,353 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F67CBA-A2D3-4F16-9F8B-66B0819D0C87}">
+  <dimension ref="B1:D35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D27F1F2-712E-47D9-BC69-378CDB4CC58B}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050C317C976D20248B2F2319776EEFE25" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8993fee6b198befc2204ddd81fef0fa7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c034aa5dba7f0148a6f00ccec9268c65" ns3:_="">
     <xsd:import namespace="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a"/>
@@ -2945,22 +3499,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C996469-9602-46C4-975E-F1E67202F6A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4BB2F41-FFF6-4C09-B8CF-7D68008AEBB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA3FD59B-64EE-4DD5-9694-E1D77FBE1C36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2976,28 +3539,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4BB2F41-FFF6-4C09-B8CF-7D68008AEBB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C996469-9602-46C4-975E-F1E67202F6A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix(logs/analysis.xlsx): added istruction set
</commit_message>
<xml_diff>
--- a/logs/analysis.xlsx
+++ b/logs/analysis.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Not Sycned\tools_notsynced\shared-ubuntu64_22-04\aurora\aurora\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04138251-22EB-46C3-9595-EA28E42E1553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA4857EF-B220-472C-86E1-B282CEEB5547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF379C5B-85D5-4F73-801D-DB5F675D5241}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DF379C5B-85D5-4F73-801D-DB5F675D5241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="instructionsetsupported" sheetId="4" r:id="rId2"/>
+    <sheet name="Resourceutilization" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="fedora_results" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$4:$E$165</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="355">
   <si>
     <t>Location             Delay type         Delay(ns)  Physical Resource</t>
   </si>
@@ -750,13 +754,367 @@
   </si>
   <si>
     <t>going to adder1, IDEX, bralu</t>
+  </si>
+  <si>
+    <t>Number of wires:                 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of wire bits:            796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of public wires:           7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of public wire bits:     270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of memories:               0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of memory bits:            0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of processes:              0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Number of cells:                 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $add                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $and                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $eq                             9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $logic_not                      1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $lt                             2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $mux                            2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $or                             1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $pmux                           1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $shl                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $shr                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $sshr                           1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $sub                            1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     $xor                            1</t>
+  </si>
+  <si>
+    <t>alu_64_bit.v</t>
+  </si>
+  <si>
+    <t>=== alu_64_bit_slim ===</t>
+  </si>
+  <si>
+    <t>   Number of wires:                 33</t>
+  </si>
+  <si>
+    <t>   Number of wire bits:            794</t>
+  </si>
+  <si>
+    <t>   Number of public wires:          15</t>
+  </si>
+  <si>
+    <t>   Number of public wire bits:     398</t>
+  </si>
+  <si>
+    <t>   Number of memories:               0</t>
+  </si>
+  <si>
+    <t>   Number of memory bits:            0</t>
+  </si>
+  <si>
+    <t>   Number of processes:              0</t>
+  </si>
+  <si>
+    <t>   Number of cells:                 87</t>
+  </si>
+  <si>
+    <t>     $and                            1</t>
+  </si>
+  <si>
+    <t>     $eq                             9</t>
+  </si>
+  <si>
+    <t>     $logic_not                      1</t>
+  </si>
+  <si>
+    <t>     $mux                            1</t>
+  </si>
+  <si>
+    <t>     $not                            1</t>
+  </si>
+  <si>
+    <t>     $or                             1</t>
+  </si>
+  <si>
+    <t>     $pmux                           1</t>
+  </si>
+  <si>
+    <t>     $reduce_or                      2</t>
+  </si>
+  <si>
+    <t>     $shl                            1</t>
+  </si>
+  <si>
+    <t>     $shr                            1</t>
+  </si>
+  <si>
+    <t>     $sshr                           1</t>
+  </si>
+  <si>
+    <t>     $xor                            3</t>
+  </si>
+  <si>
+    <t>     structuraladd_sub              64</t>
+  </si>
+  <si>
+    <t>== structuraladd_sub ===</t>
+  </si>
+  <si>
+    <t>   Number of wires:                  9</t>
+  </si>
+  <si>
+    <t>   Number of wire bits:             10</t>
+  </si>
+  <si>
+    <t>   Number of public wires:           7</t>
+  </si>
+  <si>
+    <t>   Number of public wire bits:       7</t>
+  </si>
+  <si>
+    <t>   Number of cells:                  4</t>
+  </si>
+  <si>
+    <t>     $add                            2</t>
+  </si>
+  <si>
+    <t>Original ALU</t>
+  </si>
+  <si>
+    <t>Modified ALU</t>
+  </si>
+  <si>
+    <t>Logic Utilization: Number of 4 input LUTs</t>
+  </si>
+  <si>
+    <t>Logic Distribution: Number of occupied Slices</t>
+  </si>
+  <si>
+    <t>Logic Distribution: Total Number of 4 input LUTs</t>
+  </si>
+  <si>
+    <t>ALU with Br</t>
+  </si>
+  <si>
+    <t>Logic Utilization: Number of Slice Flip Flops</t>
+  </si>
+  <si>
+    <t>UDP Only</t>
+  </si>
+  <si>
+    <t>S.no</t>
+  </si>
+  <si>
+    <t>RV64I Base Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instruction </t>
+  </si>
+  <si>
+    <t>31               27        26     25</t>
+  </si>
+  <si>
+    <t>24        20</t>
+  </si>
+  <si>
+    <t>19        15</t>
+  </si>
+  <si>
+    <t>14        12</t>
+  </si>
+  <si>
+    <t>11                 7</t>
+  </si>
+  <si>
+    <t>6             0</t>
+  </si>
+  <si>
+    <t>R-type</t>
+  </si>
+  <si>
+    <t>funct7</t>
+  </si>
+  <si>
+    <t>rs2</t>
+  </si>
+  <si>
+    <t>rs1</t>
+  </si>
+  <si>
+    <t>funct3</t>
+  </si>
+  <si>
+    <t>rd</t>
+  </si>
+  <si>
+    <t>opcode</t>
+  </si>
+  <si>
+    <t>I-type</t>
+  </si>
+  <si>
+    <t>imm[11:0]</t>
+  </si>
+  <si>
+    <t>S-type</t>
+  </si>
+  <si>
+    <t>imm[11:5]</t>
+  </si>
+  <si>
+    <t>imm[4:0]</t>
+  </si>
+  <si>
+    <t>B-type</t>
+  </si>
+  <si>
+    <t>imm[12|10:5]</t>
+  </si>
+  <si>
+    <t>imm[4:1|11]</t>
+  </si>
+  <si>
+    <t>U-type</t>
+  </si>
+  <si>
+    <t>imm[31:12]</t>
+  </si>
+  <si>
+    <t>J-type</t>
+  </si>
+  <si>
+    <t>imm[20|10:1|11|19:12]</t>
+  </si>
+  <si>
+    <t>Mnemonic</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>BNE</t>
+  </si>
+  <si>
+    <t>BLT</t>
+  </si>
+  <si>
+    <t>BGE</t>
+  </si>
+  <si>
+    <t>BLTU</t>
+  </si>
+  <si>
+    <t>BGEU</t>
+  </si>
+  <si>
+    <t>JAL</t>
+  </si>
+  <si>
+    <t>JALR</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>ADDI</t>
+  </si>
+  <si>
+    <t>SLTI</t>
+  </si>
+  <si>
+    <t>SLTIU</t>
+  </si>
+  <si>
+    <t>XORI</t>
+  </si>
+  <si>
+    <t>ORI</t>
+  </si>
+  <si>
+    <t>ANDI</t>
+  </si>
+  <si>
+    <t>SLLI</t>
+  </si>
+  <si>
+    <t>shamt</t>
+  </si>
+  <si>
+    <t>SRLI</t>
+  </si>
+  <si>
+    <t>SRAI</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>SLL</t>
+  </si>
+  <si>
+    <t>SLT</t>
+  </si>
+  <si>
+    <t>SLTU</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AND </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,16 +1122,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -781,12 +1157,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,6 +1247,1121 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fedora_results!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UDP Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fedora_results!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Logic Utilization: Number of Slice Flip Flops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logic Utilization: Number of 4 input LUTs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logic Distribution: Number of occupied Slices</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logic Distribution: Total Number of 4 input LUTs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fedora_results!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20586</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-188A-4089-9B46-FD01C3C7D2DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fedora_results!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Original ALU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fedora_results!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Logic Utilization: Number of Slice Flip Flops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logic Utilization: Number of 4 input LUTs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logic Distribution: Number of occupied Slices</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logic Distribution: Total Number of 4 input LUTs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fedora_results!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20545</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-188A-4089-9B46-FD01C3C7D2DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fedora_results!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Modified ALU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fedora_results!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Logic Utilization: Number of Slice Flip Flops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logic Utilization: Number of 4 input LUTs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logic Distribution: Number of occupied Slices</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logic Distribution: Total Number of 4 input LUTs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fedora_results!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20543</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14542</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21766</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-188A-4089-9B46-FD01C3C7D2DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fedora_results!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ALU with Br</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fedora_results!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Logic Utilization: Number of Slice Flip Flops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logic Utilization: Number of 4 input LUTs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logic Distribution: Number of occupied Slices</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logic Distribution: Total Number of 4 input LUTs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fedora_results!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20545</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14270</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21769</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-188A-4089-9B46-FD01C3C7D2DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1828890256"/>
+        <c:axId val="1828885680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1828890256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1828885680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1828885680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1828890256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46CB649C-1EB0-D5F7-CD5A-41F605E95438}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1103,7 +2663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58415AEC-B408-4D3D-935C-9A3C607B29F3}">
   <dimension ref="B2:Z165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -2813,7 +4373,1414 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DDC139-8C7A-4A00-96A6-6EC0AA413A73}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1100011</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1100011</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F11" s="3">
+        <v>100</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1100011</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" s="3">
+        <v>101</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1100011</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F13" s="3">
+        <v>110</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1100011</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F14" s="3">
+        <v>111</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1100011</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1101111</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1100111</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F17" s="3">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H17" s="3">
+        <v>100011</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F18" s="3">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H18" s="3">
+        <v>11</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>11</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H19" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F20" s="3">
+        <v>10</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H20" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F21" s="3">
+        <v>11</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H21" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F22" s="3">
+        <v>100</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H22" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>15</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F23" s="3">
+        <v>110</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H23" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F24" s="3">
+        <v>111</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H24" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H25" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F26" s="3">
+        <v>101</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H26" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>19</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C27" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F27" s="3">
+        <v>101</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H27" s="3">
+        <v>10011</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>20</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H28" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>21</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C29" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H29" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>22</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H30" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>23</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F31" s="3">
+        <v>10</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H31" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>24</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F32" s="3">
+        <v>11</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H32" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>25</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F33" s="3">
+        <v>100</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H33" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>26</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F34" s="3">
+        <v>101</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H34" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>27</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C35" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F35" s="3">
+        <v>101</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H35" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>28</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F36" s="3">
+        <v>110</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H36" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>29</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F37" s="3">
+        <v>111</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H37" s="3">
+        <v>110011</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F67CBA-A2D3-4F16-9F8B-66B0819D0C87}">
+  <dimension ref="B1:D35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D27F1F2-712E-47D9-BC69-378CDB4CC58B}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2">
+        <v>14097</v>
+      </c>
+      <c r="C2">
+        <v>14097</v>
+      </c>
+      <c r="D2">
+        <v>14097</v>
+      </c>
+      <c r="E2">
+        <v>14097</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3">
+        <v>20586</v>
+      </c>
+      <c r="C3">
+        <v>20545</v>
+      </c>
+      <c r="D3">
+        <v>20543</v>
+      </c>
+      <c r="E3">
+        <v>20545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4">
+        <v>14100</v>
+      </c>
+      <c r="C4">
+        <v>14606</v>
+      </c>
+      <c r="D4">
+        <v>14542</v>
+      </c>
+      <c r="E4">
+        <v>14270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5">
+        <v>21811</v>
+      </c>
+      <c r="C5">
+        <v>21768</v>
+      </c>
+      <c r="D5">
+        <v>21766</v>
+      </c>
+      <c r="E5">
+        <v>21769</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050C317C976D20248B2F2319776EEFE25" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8993fee6b198befc2204ddd81fef0fa7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c034aa5dba7f0148a6f00ccec9268c65" ns3:_="">
     <xsd:import namespace="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a"/>
@@ -2945,7 +5912,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2954,13 +5921,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C996469-9602-46C4-975E-F1E67202F6A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA3FD59B-64EE-4DD5-9694-E1D77FBE1C36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2978,26 +5955,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4BB2F41-FFF6-4C09-B8CF-7D68008AEBB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C996469-9602-46C4-975E-F1E67202F6A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d6c9d4c7-c0ec-4217-afa0-739e1bf9f48a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>